<commit_message>
added attitional markdowns with more information
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfine\Desktop\algorithms project\COMP257-Algorithms-Project\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD61BAF6-0BF1-45BB-AD5D-1D25DEA18508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0527461B-F056-4203-8ADD-E0C0EAD79846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="661" firstSheet="4" activeTab="8" xr2:uid="{10AED6EE-AB06-4515-9E7E-31A2B38653FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="661" firstSheet="2" activeTab="5" xr2:uid="{10AED6EE-AB06-4515-9E7E-31A2B38653FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Brute Force" sheetId="1" r:id="rId1"/>
@@ -31980,8 +31980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801C8948-40CF-4A6D-9616-1695B7F9F400}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32245,8 +32245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567CEADA-61F2-4600-B967-3BEFDA08F01D}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33006,8 +33006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB749836-97DE-4E49-8957-FDF8015D0014}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>